<commit_message>
new test case for OCI CU was added
</commit_message>
<xml_diff>
--- a/TestData/addVcenter.xlsx
+++ b/TestData/addVcenter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786DB4AC-25BC-45A8-BC95-E3BA73E9C902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C7A886-B5CA-4954-ADFB-0FB9CA64141B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,66 @@
   </si>
   <si>
     <t>Port</t>
+  </si>
+  <si>
+    <t>Common Data</t>
+  </si>
+  <si>
+    <t>Cluster Name</t>
+  </si>
+  <si>
+    <t>ESX Host</t>
+  </si>
+  <si>
+    <t>Datastore</t>
+  </si>
+  <si>
+    <t>Device Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Network Name</t>
+  </si>
+  <si>
+    <t>DHCP / Static IP</t>
+  </si>
+  <si>
+    <t>CIDR</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>DNS1</t>
+  </si>
+  <si>
+    <t>DNS2</t>
+  </si>
+  <si>
+    <t>VM Folder</t>
+  </si>
+  <si>
+    <t>Resource Pool</t>
+  </si>
+  <si>
+    <t>Routes</t>
+  </si>
+  <si>
+    <t>NIC's</t>
+  </si>
+  <si>
+    <t>Edit Wave</t>
+  </si>
+  <si>
+    <t>Wave Name</t>
+  </si>
+  <si>
+    <t>Autoprovision</t>
+  </si>
+  <si>
+    <t>Environment</t>
   </si>
 </sst>
 </file>
@@ -83,9 +143,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,38 +435,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>